<commit_message>
added code for wk3
</commit_message>
<xml_diff>
--- a/devasc_studyplan.xlsx
+++ b/devasc_studyplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10409"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/dev/DEVASC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA84D25D-078B-8845-8FA0-E266266A750D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21F1419-48BD-7746-AF33-25BC3AF0AA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4060" yWindow="760" windowWidth="24720" windowHeight="17800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="306">
   <si>
     <t>Important notes</t>
   </si>
@@ -1679,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2122,6 +2122,9 @@
       <c r="E27" s="6">
         <v>2.4</v>
       </c>
+      <c r="F27" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
@@ -2136,6 +2139,9 @@
       <c r="E28" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="F28" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
@@ -2150,6 +2156,9 @@
       <c r="E29" s="6" t="s">
         <v>51</v>
       </c>
+      <c r="F29" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
@@ -2164,6 +2173,9 @@
       <c r="E30" s="6" t="s">
         <v>51</v>
       </c>
+      <c r="F30" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
@@ -2178,6 +2190,9 @@
       <c r="E31" s="6" t="s">
         <v>191</v>
       </c>
+      <c r="F31" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" s="7" t="s">
@@ -2192,8 +2207,11 @@
       <c r="E32" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>247</v>
       </c>
@@ -2206,8 +2224,11 @@
       <c r="E33" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>248</v>
       </c>
@@ -2220,8 +2241,11 @@
       <c r="E34" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>41</v>
       </c>
@@ -2234,8 +2258,11 @@
       <c r="E35" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>273</v>
       </c>
@@ -2249,7 +2276,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>4</v>
       </c>
@@ -2266,7 +2293,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>48</v>
       </c>
@@ -2280,7 +2307,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>75</v>
       </c>
@@ -2294,7 +2321,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>75</v>
       </c>
@@ -2308,7 +2335,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>75</v>
       </c>
@@ -2322,7 +2349,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>75</v>
       </c>
@@ -2336,7 +2363,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>47</v>
       </c>
@@ -2350,7 +2377,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" s="7" t="s">
         <v>49</v>
       </c>
@@ -2364,7 +2391,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>76</v>
       </c>
@@ -2378,7 +2405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>76</v>
       </c>
@@ -2392,7 +2419,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>76</v>
       </c>

</xml_diff>